<commit_message>
OCXO V3 BOM change
1. Changing OCXO V3 BOM default to use single ended from baseboard, instead of differential.
2. Adding a no oscillator version for a generic board for manual soldering in lab
</commit_message>
<xml_diff>
--- a/Time-Card/OSC/OCXO Daughtercard/BOM/Abracon_AOCJYR_bom.xlsx
+++ b/Time-Card/OSC/OCXO Daughtercard/BOM/Abracon_AOCJYR_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julianstj\Desktop\WorkNotes\Projects\PTP\Time-Appliance-Project-master\Time-Card\OSC\OCXO Daughtercard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F6096-65CD-42B2-82CE-070123591C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032FE9C8-2A59-4A57-B6F3-CC122476CACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2D3E0BFC-5E22-4D76-99F4-CFC4E352CD26}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D3E0BFC-5E22-4D76-99F4-CFC4E352CD26}"/>
   </bookViews>
   <sheets>
     <sheet name="845-02233-03-RevX1_bom" sheetId="1" r:id="rId1"/>
@@ -443,9 +443,6 @@
     <t>2363481</t>
   </si>
   <si>
-    <t>R17, R18, R19, R24, R25, R26, R29, R31</t>
-  </si>
-  <si>
     <t>R27, R28</t>
   </si>
   <si>
@@ -636,6 +633,9 @@
   </si>
   <si>
     <t>SITIME_SPL-086-CQFN-010-C07050_REV_DRAFT</t>
+  </si>
+  <si>
+    <t>R17, R18, R19, R24, R25, R26, R30, R32</t>
   </si>
 </sst>
 </file>
@@ -1014,13 +1014,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97BCE83-2F52-4575-90D4-06189B3D219C}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
     <col min="2" max="2" width="37.90625" customWidth="1"/>
     <col min="3" max="3" width="21.54296875" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" customWidth="1"/>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>86</v>
@@ -1891,16 +1891,16 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1912,31 +1912,31 @@
         <v>131</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1948,10 +1948,10 @@
         <v>131</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>42</v>
@@ -1960,21 +1960,21 @@
         <v>10</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -1984,11 +1984,11 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>10</v>
@@ -1997,16 +1997,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2016,11 +2016,11 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>10</v>
@@ -2029,16 +2029,16 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2048,11 +2048,11 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>10</v>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -2080,11 +2080,11 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>10</v>
@@ -2093,16 +2093,16 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -2112,11 +2112,11 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>10</v>
@@ -2125,16 +2125,16 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -2144,7 +2144,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>32</v>
@@ -2153,16 +2153,16 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -2172,7 +2172,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>32</v>
@@ -2181,16 +2181,16 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -2200,11 +2200,11 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>10</v>
@@ -2213,16 +2213,16 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2232,7 +2232,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>32</v>
@@ -2241,16 +2241,16 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -2260,7 +2260,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>10</v>

</xml_diff>